<commit_message>
Fixed thresholds and North Macedonia
</commit_message>
<xml_diff>
--- a/src/data/overview.xlsx
+++ b/src/data/overview.xlsx
@@ -514,7 +514,7 @@
     <t xml:space="preserve">Sunrg softver i IT solucii</t>
   </si>
   <si>
-    <t xml:space="preserve">Macedonia</t>
+    <t xml:space="preserve">North Macedonia</t>
   </si>
   <si>
     <t xml:space="preserve">VAE BV</t>
@@ -1782,7 +1782,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="S17" activeCellId="0" sqref="S17"/>
+      <selection pane="bottomLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>